<commit_message>
[LPF-996]: Fix CCMS and CIS Bank Account Report w Category Code (YTD)
</commit_message>
<xml_diff>
--- a/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
+++ b/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
@@ -7,14 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Transparency Rec" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="By Source and Expenditure type" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Transparency Rec" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary'!$B$5:$D$8</definedName>
   </definedNames>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache cacheId="240" r:id="rId3"/>
+    <pivotCache cacheId="240" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -132458,6 +132459,141 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SourceNType" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="0" colGrandTotals="0" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="1" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
+  <location ref="A5:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="4"/>
+  <pivotFields count="12">
+    <pivotField name="Source " axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="0">
+      <items count="3">
+        <item t="data" h="1" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" h="1" sd="1" x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Expenditure Type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="4">
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Month" axis="axisCol" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="24">
+        <item t="data" sd="1" m="1" x="22"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" m="1" x="21"/>
+        <item t="data" sd="1" m="1" x="20"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="11"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="9"/>
+        <item t="data" sd="1" m="1" x="10"/>
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField name="Expenditure sub type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="8">
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Description" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="48">
+        <item t="data" sd="1" m="1" x="30"/>
+        <item t="data" sd="1" m="1" x="24"/>
+        <item t="data" sd="1" m="1" x="31"/>
+        <item t="data" sd="1" m="1" x="42"/>
+        <item t="data" sd="1" m="1" x="32"/>
+        <item t="data" sd="1" m="1" x="9"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="29"/>
+        <item t="data" sd="1" m="1" x="21"/>
+        <item t="data" sd="1" m="1" x="33"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="23"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="35"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="26"/>
+        <item t="data" sd="1" m="1" x="27"/>
+        <item t="data" sd="1" m="1" x="22"/>
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="20"/>
+        <item t="data" sd="1" m="1" x="10"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" m="1" x="25"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="28"/>
+        <item t="data" sd="1" m="1" x="11"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="36"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" m="1" x="43"/>
+        <item t="data" sd="1" m="1" x="38"/>
+        <item t="data" sd="1" m="1" x="39"/>
+        <item t="data" sd="1" m="1" x="41"/>
+        <item t="data" sd="1" m="1" x="46"/>
+        <item t="data" sd="1" m="1" x="34"/>
+        <item t="data" sd="1" m="1" x="40"/>
+        <item t="data" sd="1" m="1" x="37"/>
+        <item t="data" sd="1" m="1" x="44"/>
+        <item t="data" sd="1" m="1" x="45"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField dataField="1" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="2"/>
+    <field x="5"/>
+    <field x="8"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="11" subtotal="sum" showDataAs="normal" baseField="8" baseItem="33" numFmtId="8"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Transparency rec pivot" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
   <location ref="A5:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
@@ -132985,6 +133121,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet4">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="21.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="22.5" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" min="6" max="7"/>
+    <col width="11.83203125" customWidth="1" min="8" max="10"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="13.5" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="12.6640625" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" min="14" max="17"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Sum of Amount</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Source </t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>Expenditure Type</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>Expenditure sub type</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>

</xml_diff>

<commit_message>
[LPF-879]: CCMS Third party report
Signed-off-by: robert.buczek <robert.buczek@digital.justice.gov.uk>
</commit_message>
<xml_diff>
--- a/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
+++ b/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
@@ -7,17 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="By Source and Expenditure type" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Provider Contigency" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Transparency Rec" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="MAIN" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Transparency Rec" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary'!$B$5:$D$8</definedName>
   </definedNames>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache cacheId="240" r:id="rId6"/>
+    <pivotCache cacheId="240" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -132461,141 +132458,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SourceNType" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="0" colGrandTotals="0" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="1" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
-  <location ref="A5:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="4"/>
-  <pivotFields count="12">
-    <pivotField name="Source " axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="0">
-      <items count="3">
-        <item t="data" h="1" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" h="1" sd="1" x="0"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField name="Expenditure Type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="4">
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField name="Month" axis="axisCol" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="24">
-        <item t="data" sd="1" m="1" x="22"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="data" sd="1" m="1" x="21"/>
-        <item t="data" sd="1" m="1" x="20"/>
-        <item t="data" sd="1" m="1" x="12"/>
-        <item t="data" sd="1" m="1" x="18"/>
-        <item t="data" sd="1" m="1" x="13"/>
-        <item t="data" sd="1" m="1" x="19"/>
-        <item t="data" sd="1" m="1" x="11"/>
-        <item t="data" sd="1" m="1" x="15"/>
-        <item t="data" sd="1" m="1" x="16"/>
-        <item t="data" sd="1" m="1" x="17"/>
-        <item t="data" sd="1" m="1" x="14"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="4"/>
-        <item t="data" sd="1" m="1" x="5"/>
-        <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="7"/>
-        <item t="data" sd="1" m="1" x="8"/>
-        <item t="data" sd="1" m="1" x="9"/>
-        <item t="data" sd="1" m="1" x="10"/>
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField name="Expenditure sub type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="8">
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="4"/>
-        <item t="data" sd="1" m="1" x="5"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField name="Description" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="48">
-        <item t="data" sd="1" m="1" x="30"/>
-        <item t="data" sd="1" m="1" x="24"/>
-        <item t="data" sd="1" m="1" x="31"/>
-        <item t="data" sd="1" m="1" x="42"/>
-        <item t="data" sd="1" m="1" x="32"/>
-        <item t="data" sd="1" m="1" x="9"/>
-        <item t="data" sd="1" m="1" x="12"/>
-        <item t="data" sd="1" m="1" x="5"/>
-        <item t="data" sd="1" m="1" x="29"/>
-        <item t="data" sd="1" m="1" x="21"/>
-        <item t="data" sd="1" m="1" x="33"/>
-        <item t="data" sd="1" m="1" x="19"/>
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="23"/>
-        <item t="data" sd="1" m="1" x="15"/>
-        <item t="data" sd="1" m="1" x="17"/>
-        <item t="data" sd="1" m="1" x="35"/>
-        <item t="data" sd="1" m="1" x="16"/>
-        <item t="data" sd="1" m="1" x="26"/>
-        <item t="data" sd="1" m="1" x="27"/>
-        <item t="data" sd="1" m="1" x="22"/>
-        <item t="data" sd="1" m="1" x="13"/>
-        <item t="data" sd="1" m="1" x="4"/>
-        <item t="data" sd="1" m="1" x="20"/>
-        <item t="data" sd="1" m="1" x="10"/>
-        <item t="data" sd="1" m="1" x="14"/>
-        <item t="data" sd="1" m="1" x="18"/>
-        <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="25"/>
-        <item t="data" sd="1" m="1" x="7"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="28"/>
-        <item t="data" sd="1" m="1" x="11"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="8"/>
-        <item t="data" sd="1" m="1" x="36"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="data" sd="1" m="1" x="43"/>
-        <item t="data" sd="1" m="1" x="38"/>
-        <item t="data" sd="1" m="1" x="39"/>
-        <item t="data" sd="1" m="1" x="41"/>
-        <item t="data" sd="1" m="1" x="46"/>
-        <item t="data" sd="1" m="1" x="34"/>
-        <item t="data" sd="1" m="1" x="40"/>
-        <item t="data" sd="1" m="1" x="37"/>
-        <item t="data" sd="1" m="1" x="44"/>
-        <item t="data" sd="1" m="1" x="45"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField dataField="1" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="0"/>
-    <field x="2"/>
-    <field x="5"/>
-    <field x="8"/>
-  </rowFields>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <dataFields count="1">
-    <dataField name="Sum of Amount" fld="11" subtotal="sum" showDataAs="normal" baseField="8" baseItem="33" numFmtId="8"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Transparency rec pivot" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
   <location ref="A5:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
@@ -133123,174 +132985,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet4">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A5:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="21.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="22.5" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="12.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="6" max="7"/>
-    <col width="11.83203125" customWidth="1" min="8" max="10"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="13.5" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="12.6640625" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="14" max="17"/>
-  </cols>
-  <sheetData>
-    <row r="5">
-      <c r="A5" s="11" t="inlineStr">
-        <is>
-          <t>Sum of Amount</t>
-        </is>
-      </c>
-      <c r="E5" s="11" t="inlineStr">
-        <is>
-          <t>Month</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Source </t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>Expenditure Type</t>
-        </is>
-      </c>
-      <c r="C6" s="11" t="inlineStr">
-        <is>
-          <t>Expenditure sub type</t>
-        </is>
-      </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet13">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD11967"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="15.5" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="67.5" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10.83203125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="21.1640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="66.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="26" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="21.5" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="19.1640625" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="23.6640625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="8.1640625" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="12.5" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="9.83203125" bestFit="1" customWidth="1" min="13" max="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1" s="16">
-      <c r="A1" s="16" t="inlineStr">
-        <is>
-          <t>OFFICE_NUMBER</t>
-        </is>
-      </c>
-      <c r="B1" s="16" t="inlineStr">
-        <is>
-          <t>OFFICE_NAME</t>
-        </is>
-      </c>
-      <c r="C1" s="16" t="inlineStr">
-        <is>
-          <t>BANK_NUM</t>
-        </is>
-      </c>
-      <c r="D1" s="16" t="inlineStr">
-        <is>
-          <t>BANK_ACCOUNT_NUM</t>
-        </is>
-      </c>
-      <c r="E1" s="16" t="inlineStr">
-        <is>
-          <t>BANK_ACCOUNT_NAME</t>
-        </is>
-      </c>
-      <c r="F1" s="16" t="inlineStr">
-        <is>
-          <t>VENDOR_SITE_ID</t>
-        </is>
-      </c>
-      <c r="G1" s="16" t="inlineStr">
-        <is>
-          <t>HOLD_ALL_PAYMENTS_FLAG</t>
-        </is>
-      </c>
-      <c r="H1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENTS_CHECKSUM</t>
-        </is>
-      </c>
-      <c r="I1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENTS_LAST_SIX</t>
-        </is>
-      </c>
-      <c r="J1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENTS_LAST_TWELVE</t>
-        </is>
-      </c>
-      <c r="K1" s="16" t="inlineStr">
-        <is>
-          <t>AVG_SIX</t>
-        </is>
-      </c>
-      <c r="L1" s="16" t="inlineStr">
-        <is>
-          <t>AVG_TWELVE</t>
-        </is>
-      </c>
-      <c r="M1" s="16" t="inlineStr">
-        <is>
-          <t>AR_DEBT</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -133365,100 +133059,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet2">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD1014"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="7.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="11.6640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="17.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="16.83203125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="7.5" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="18.5" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="35.6640625" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="9.5" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="18.1640625" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="12" max="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1" s="16">
-      <c r="A1" s="16" t="inlineStr">
-        <is>
-          <t>SOURCE</t>
-        </is>
-      </c>
-      <c r="B1" s="16" t="inlineStr">
-        <is>
-          <t>INV_SOURCE</t>
-        </is>
-      </c>
-      <c r="C1" s="16" t="inlineStr">
-        <is>
-          <t>SUB_SOURCE</t>
-        </is>
-      </c>
-      <c r="D1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENT_DATE</t>
-        </is>
-      </c>
-      <c r="E1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENT_MONTH</t>
-        </is>
-      </c>
-      <c r="F1" s="16" t="inlineStr">
-        <is>
-          <t>SETTLEMENT_TYPE</t>
-        </is>
-      </c>
-      <c r="G1" s="16" t="inlineStr">
-        <is>
-          <t>SCHEME</t>
-        </is>
-      </c>
-      <c r="H1" s="16" t="inlineStr">
-        <is>
-          <t>SUB_SCHEME</t>
-        </is>
-      </c>
-      <c r="I1" s="16" t="inlineStr">
-        <is>
-          <t>DETAIL_DESC</t>
-        </is>
-      </c>
-      <c r="J1" s="16" t="inlineStr">
-        <is>
-          <t>CAT_CODE</t>
-        </is>
-      </c>
-      <c r="K1" s="16" t="inlineStr">
-        <is>
-          <t>AP_AR_MOVEMENT</t>
-        </is>
-      </c>
-      <c r="L1" s="16" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[LPF-879]: CCMS Third party report (#257)
Signed-off-by: robert.buczek <robert.buczek@digital.justice.gov.uk>
</commit_message>
<xml_diff>
--- a/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
+++ b/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
@@ -7,17 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="By Source and Expenditure type" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Provider Contigency" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Transparency Rec" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="MAIN" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Transparency Rec" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary'!$B$5:$D$8</definedName>
   </definedNames>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache cacheId="240" r:id="rId6"/>
+    <pivotCache cacheId="240" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -132461,141 +132458,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SourceNType" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="0" colGrandTotals="0" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="1" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
-  <location ref="A5:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="4"/>
-  <pivotFields count="12">
-    <pivotField name="Source " axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="0">
-      <items count="3">
-        <item t="data" h="1" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" h="1" sd="1" x="0"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField name="Expenditure Type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="4">
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField name="Month" axis="axisCol" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="24">
-        <item t="data" sd="1" m="1" x="22"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="data" sd="1" m="1" x="21"/>
-        <item t="data" sd="1" m="1" x="20"/>
-        <item t="data" sd="1" m="1" x="12"/>
-        <item t="data" sd="1" m="1" x="18"/>
-        <item t="data" sd="1" m="1" x="13"/>
-        <item t="data" sd="1" m="1" x="19"/>
-        <item t="data" sd="1" m="1" x="11"/>
-        <item t="data" sd="1" m="1" x="15"/>
-        <item t="data" sd="1" m="1" x="16"/>
-        <item t="data" sd="1" m="1" x="17"/>
-        <item t="data" sd="1" m="1" x="14"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="4"/>
-        <item t="data" sd="1" m="1" x="5"/>
-        <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="7"/>
-        <item t="data" sd="1" m="1" x="8"/>
-        <item t="data" sd="1" m="1" x="9"/>
-        <item t="data" sd="1" m="1" x="10"/>
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField name="Expenditure sub type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="8">
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="4"/>
-        <item t="data" sd="1" m="1" x="5"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField name="Description" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
-      <items count="48">
-        <item t="data" sd="1" m="1" x="30"/>
-        <item t="data" sd="1" m="1" x="24"/>
-        <item t="data" sd="1" m="1" x="31"/>
-        <item t="data" sd="1" m="1" x="42"/>
-        <item t="data" sd="1" m="1" x="32"/>
-        <item t="data" sd="1" m="1" x="9"/>
-        <item t="data" sd="1" m="1" x="12"/>
-        <item t="data" sd="1" m="1" x="5"/>
-        <item t="data" sd="1" m="1" x="29"/>
-        <item t="data" sd="1" m="1" x="21"/>
-        <item t="data" sd="1" m="1" x="33"/>
-        <item t="data" sd="1" m="1" x="19"/>
-        <item t="data" sd="1" m="1" x="1"/>
-        <item t="data" sd="1" m="1" x="23"/>
-        <item t="data" sd="1" m="1" x="15"/>
-        <item t="data" sd="1" m="1" x="17"/>
-        <item t="data" sd="1" m="1" x="35"/>
-        <item t="data" sd="1" m="1" x="16"/>
-        <item t="data" sd="1" m="1" x="26"/>
-        <item t="data" sd="1" m="1" x="27"/>
-        <item t="data" sd="1" m="1" x="22"/>
-        <item t="data" sd="1" m="1" x="13"/>
-        <item t="data" sd="1" m="1" x="4"/>
-        <item t="data" sd="1" m="1" x="20"/>
-        <item t="data" sd="1" m="1" x="10"/>
-        <item t="data" sd="1" m="1" x="14"/>
-        <item t="data" sd="1" m="1" x="18"/>
-        <item t="data" sd="1" m="1" x="6"/>
-        <item t="data" sd="1" m="1" x="25"/>
-        <item t="data" sd="1" m="1" x="7"/>
-        <item t="data" sd="1" m="1" x="2"/>
-        <item t="data" sd="1" m="1" x="28"/>
-        <item t="data" sd="1" m="1" x="11"/>
-        <item t="data" sd="1" m="1" x="3"/>
-        <item t="data" sd="1" m="1" x="8"/>
-        <item t="data" sd="1" m="1" x="36"/>
-        <item t="data" sd="1" x="0"/>
-        <item t="data" sd="1" m="1" x="43"/>
-        <item t="data" sd="1" m="1" x="38"/>
-        <item t="data" sd="1" m="1" x="39"/>
-        <item t="data" sd="1" m="1" x="41"/>
-        <item t="data" sd="1" m="1" x="46"/>
-        <item t="data" sd="1" m="1" x="34"/>
-        <item t="data" sd="1" m="1" x="40"/>
-        <item t="data" sd="1" m="1" x="37"/>
-        <item t="data" sd="1" m="1" x="44"/>
-        <item t="data" sd="1" m="1" x="45"/>
-        <item t="default" sd="1"/>
-      </items>
-    </pivotField>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-    <pivotField dataField="1" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
-  </pivotFields>
-  <rowFields count="4">
-    <field x="0"/>
-    <field x="2"/>
-    <field x="5"/>
-    <field x="8"/>
-  </rowFields>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <dataFields count="1">
-    <dataField name="Sum of Amount" fld="11" subtotal="sum" showDataAs="normal" baseField="8" baseItem="33" numFmtId="8"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Transparency rec pivot" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
   <location ref="A5:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
@@ -133123,174 +132985,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet4">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A5:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="21.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="22.5" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="12.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="6" max="7"/>
-    <col width="11.83203125" customWidth="1" min="8" max="10"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="13.5" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="12.6640625" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="14" max="17"/>
-  </cols>
-  <sheetData>
-    <row r="5">
-      <c r="A5" s="11" t="inlineStr">
-        <is>
-          <t>Sum of Amount</t>
-        </is>
-      </c>
-      <c r="E5" s="11" t="inlineStr">
-        <is>
-          <t>Month</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Source </t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>Expenditure Type</t>
-        </is>
-      </c>
-      <c r="C6" s="11" t="inlineStr">
-        <is>
-          <t>Expenditure sub type</t>
-        </is>
-      </c>
-      <c r="D6" s="11" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet13">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD11967"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="15.5" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="67.5" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10.83203125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="21.1640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="66.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="26" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="21.5" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="19.1640625" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="23.6640625" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="8.1640625" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="12.5" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="9.83203125" bestFit="1" customWidth="1" min="13" max="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1" s="16">
-      <c r="A1" s="16" t="inlineStr">
-        <is>
-          <t>OFFICE_NUMBER</t>
-        </is>
-      </c>
-      <c r="B1" s="16" t="inlineStr">
-        <is>
-          <t>OFFICE_NAME</t>
-        </is>
-      </c>
-      <c r="C1" s="16" t="inlineStr">
-        <is>
-          <t>BANK_NUM</t>
-        </is>
-      </c>
-      <c r="D1" s="16" t="inlineStr">
-        <is>
-          <t>BANK_ACCOUNT_NUM</t>
-        </is>
-      </c>
-      <c r="E1" s="16" t="inlineStr">
-        <is>
-          <t>BANK_ACCOUNT_NAME</t>
-        </is>
-      </c>
-      <c r="F1" s="16" t="inlineStr">
-        <is>
-          <t>VENDOR_SITE_ID</t>
-        </is>
-      </c>
-      <c r="G1" s="16" t="inlineStr">
-        <is>
-          <t>HOLD_ALL_PAYMENTS_FLAG</t>
-        </is>
-      </c>
-      <c r="H1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENTS_CHECKSUM</t>
-        </is>
-      </c>
-      <c r="I1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENTS_LAST_SIX</t>
-        </is>
-      </c>
-      <c r="J1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENTS_LAST_TWELVE</t>
-        </is>
-      </c>
-      <c r="K1" s="16" t="inlineStr">
-        <is>
-          <t>AVG_SIX</t>
-        </is>
-      </c>
-      <c r="L1" s="16" t="inlineStr">
-        <is>
-          <t>AVG_TWELVE</t>
-        </is>
-      </c>
-      <c r="M1" s="16" t="inlineStr">
-        <is>
-          <t>AR_DEBT</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -133365,100 +133059,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr codeName="Sheet2">
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:L1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD1014"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col width="7.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="11.6640625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="15.33203125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="14.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="17.33203125" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="16.83203125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="7.5" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="18.5" bestFit="1" customWidth="1" min="8" max="8"/>
-    <col width="35.6640625" bestFit="1" customWidth="1" min="9" max="9"/>
-    <col width="9.5" bestFit="1" customWidth="1" min="10" max="10"/>
-    <col width="18.1640625" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="11.83203125" bestFit="1" customWidth="1" min="12" max="12"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="1" s="16">
-      <c r="A1" s="16" t="inlineStr">
-        <is>
-          <t>SOURCE</t>
-        </is>
-      </c>
-      <c r="B1" s="16" t="inlineStr">
-        <is>
-          <t>INV_SOURCE</t>
-        </is>
-      </c>
-      <c r="C1" s="16" t="inlineStr">
-        <is>
-          <t>SUB_SOURCE</t>
-        </is>
-      </c>
-      <c r="D1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENT_DATE</t>
-        </is>
-      </c>
-      <c r="E1" s="16" t="inlineStr">
-        <is>
-          <t>PAYMENT_MONTH</t>
-        </is>
-      </c>
-      <c r="F1" s="16" t="inlineStr">
-        <is>
-          <t>SETTLEMENT_TYPE</t>
-        </is>
-      </c>
-      <c r="G1" s="16" t="inlineStr">
-        <is>
-          <t>SCHEME</t>
-        </is>
-      </c>
-      <c r="H1" s="16" t="inlineStr">
-        <is>
-          <t>SUB_SCHEME</t>
-        </is>
-      </c>
-      <c r="I1" s="16" t="inlineStr">
-        <is>
-          <t>DETAIL_DESC</t>
-        </is>
-      </c>
-      <c r="J1" s="16" t="inlineStr">
-        <is>
-          <t>CAT_CODE</t>
-        </is>
-      </c>
-      <c r="K1" s="16" t="inlineStr">
-        <is>
-          <t>AP_AR_MOVEMENT</t>
-        </is>
-      </c>
-      <c r="L1" s="16" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
[LPF-996]: Fix CCMS and CIS Bank Account Report w Category Code (YTD) (#278)
</commit_message>
<xml_diff>
--- a/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
+++ b/src/main/resources/CCMS_AND_CIS_BANK_ACCOUNT_REPORT_W_CATEGORY_CODE_YTD.xlsx
@@ -7,14 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Transparency Rec" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="By Source and Expenditure type" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Transparency Rec" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Summary'!$B$5:$D$8</definedName>
   </definedNames>
   <calcPr calcId="191028" fullCalcOnLoad="1"/>
   <pivotCaches>
-    <pivotCache cacheId="240" r:id="rId3"/>
+    <pivotCache cacheId="240" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -132458,6 +132459,141 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SourceNType" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="0" colGrandTotals="0" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="1" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
+  <location ref="A5:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="4"/>
+  <pivotFields count="12">
+    <pivotField name="Source " axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="0">
+      <items count="3">
+        <item t="data" h="1" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" h="1" sd="1" x="0"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Expenditure Type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="4">
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Month" axis="axisCol" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="24">
+        <item t="data" sd="1" m="1" x="22"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" m="1" x="21"/>
+        <item t="data" sd="1" m="1" x="20"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="11"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="9"/>
+        <item t="data" sd="1" m="1" x="10"/>
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField name="Expenditure sub type" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="8">
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField name="Description" axis="axisRow" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1">
+      <items count="48">
+        <item t="data" sd="1" m="1" x="30"/>
+        <item t="data" sd="1" m="1" x="24"/>
+        <item t="data" sd="1" m="1" x="31"/>
+        <item t="data" sd="1" m="1" x="42"/>
+        <item t="data" sd="1" m="1" x="32"/>
+        <item t="data" sd="1" m="1" x="9"/>
+        <item t="data" sd="1" m="1" x="12"/>
+        <item t="data" sd="1" m="1" x="5"/>
+        <item t="data" sd="1" m="1" x="29"/>
+        <item t="data" sd="1" m="1" x="21"/>
+        <item t="data" sd="1" m="1" x="33"/>
+        <item t="data" sd="1" m="1" x="19"/>
+        <item t="data" sd="1" m="1" x="1"/>
+        <item t="data" sd="1" m="1" x="23"/>
+        <item t="data" sd="1" m="1" x="15"/>
+        <item t="data" sd="1" m="1" x="17"/>
+        <item t="data" sd="1" m="1" x="35"/>
+        <item t="data" sd="1" m="1" x="16"/>
+        <item t="data" sd="1" m="1" x="26"/>
+        <item t="data" sd="1" m="1" x="27"/>
+        <item t="data" sd="1" m="1" x="22"/>
+        <item t="data" sd="1" m="1" x="13"/>
+        <item t="data" sd="1" m="1" x="4"/>
+        <item t="data" sd="1" m="1" x="20"/>
+        <item t="data" sd="1" m="1" x="10"/>
+        <item t="data" sd="1" m="1" x="14"/>
+        <item t="data" sd="1" m="1" x="18"/>
+        <item t="data" sd="1" m="1" x="6"/>
+        <item t="data" sd="1" m="1" x="25"/>
+        <item t="data" sd="1" m="1" x="7"/>
+        <item t="data" sd="1" m="1" x="2"/>
+        <item t="data" sd="1" m="1" x="28"/>
+        <item t="data" sd="1" m="1" x="11"/>
+        <item t="data" sd="1" m="1" x="3"/>
+        <item t="data" sd="1" m="1" x="8"/>
+        <item t="data" sd="1" m="1" x="36"/>
+        <item t="data" sd="1" x="0"/>
+        <item t="data" sd="1" m="1" x="43"/>
+        <item t="data" sd="1" m="1" x="38"/>
+        <item t="data" sd="1" m="1" x="39"/>
+        <item t="data" sd="1" m="1" x="41"/>
+        <item t="data" sd="1" m="1" x="46"/>
+        <item t="data" sd="1" m="1" x="34"/>
+        <item t="data" sd="1" m="1" x="40"/>
+        <item t="data" sd="1" m="1" x="37"/>
+        <item t="data" sd="1" m="1" x="44"/>
+        <item t="data" sd="1" m="1" x="45"/>
+        <item t="default" sd="1"/>
+      </items>
+    </pivotField>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+    <pivotField dataField="1" showDropDowns="1" compact="0" outline="0" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
+  </pivotFields>
+  <rowFields count="4">
+    <field x="0"/>
+    <field x="2"/>
+    <field x="5"/>
+    <field x="8"/>
+  </rowFields>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <dataFields count="1">
+    <dataField name="Sum of Amount" fld="11" subtotal="sum" showDataAs="normal" baseField="8" baseItem="33" numFmtId="8"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Transparency rec pivot" cacheId="240" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="8" minRefreshableVersion="3" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="0" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="1" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="3" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="1" outline="1" outlineData="1" compactData="1" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" r:id="rId1">
   <location ref="A5:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="12">
@@ -132985,6 +133121,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr codeName="Sheet4">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A5:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.33203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="21.1640625" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="22.5" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="12.6640625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="9" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" min="6" max="7"/>
+    <col width="11.83203125" customWidth="1" min="8" max="10"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="13.5" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="12.6640625" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="11.83203125" bestFit="1" customWidth="1" min="14" max="17"/>
+  </cols>
+  <sheetData>
+    <row r="5">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Sum of Amount</t>
+        </is>
+      </c>
+      <c r="E5" s="11" t="inlineStr">
+        <is>
+          <t>Month</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Source </t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="inlineStr">
+        <is>
+          <t>Expenditure Type</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="inlineStr">
+        <is>
+          <t>Expenditure sub type</t>
+        </is>
+      </c>
+      <c r="D6" s="11" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet3">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>

</xml_diff>